<commit_message>
Format count with queries
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ki\mygitsrc\udemy-sql-server\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622D6994-3043-4F78-9513-35F6449D917D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="13104" yWindow="2232" windowWidth="8172" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>[tblEmployee]</t>
   </si>
@@ -73,12 +79,54 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>tblTransaction</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>smallmoney</t>
+  </si>
+  <si>
+    <t>dateoftransaction</t>
+  </si>
+  <si>
+    <t>bcs:  decimal numeric(7,2)</t>
+  </si>
+  <si>
+    <t>4 bytes</t>
+  </si>
+  <si>
+    <t>bcs:  datetime2 with sec is always zero</t>
+  </si>
+  <si>
+    <t>smalldatetime</t>
+  </si>
+  <si>
+    <t>uniquely identify an employee</t>
+  </si>
+  <si>
+    <t>SCD : slowly changing dimension</t>
+  </si>
+  <si>
+    <t>dateofbirth--possible</t>
+  </si>
+  <si>
+    <t>governmentId--but it is null-able</t>
+  </si>
+  <si>
+    <t>unique?</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,6 +167,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -167,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +251,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,6 +303,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -410,11 +495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,14 +507,21 @@
     <col min="3" max="3" width="25.5546875" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="44.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>1</v>
       </c>
@@ -439,8 +531,20 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -450,8 +554,17 @@
       <c r="E5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -461,8 +574,17 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>10</v>
       </c>
@@ -473,7 +595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>11</v>
       </c>
@@ -484,7 +606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -495,7 +617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>16</v>
       </c>
@@ -504,6 +626,24 @@
       </c>
       <c r="E10" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -524,7 +664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Primary and Foreign Key
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ki\mygitsrc\udemy-sql-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FE8CD0-643E-490D-BC30-384E5714FB98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA8F0BF-D002-48EB-9EBF-DEA65B5FD6ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1836" yWindow="636" windowWidth="11280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>[tblEmployee]</t>
   </si>
@@ -184,6 +184,33 @@
   </si>
   <si>
     <t xml:space="preserve"> not natural key</t>
+  </si>
+  <si>
+    <t>Foreign key</t>
+  </si>
+  <si>
+    <t>seek</t>
+  </si>
+  <si>
+    <t>scan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connect 2 tables </t>
+  </si>
+  <si>
+    <t>cascade effect</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>no actions</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -671,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P25"/>
+  <dimension ref="A3:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,6 +1022,47 @@
       </c>
       <c r="H25" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Views with Encryption and CheckOption
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ki\mygitsrc\udemy-sql-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D2ED67-8A83-4E64-936D-2A0CF5CDB71A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD09DA10-8DAD-4640-A52E-414D6F3B52B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11232" yWindow="1332" windowWidth="11280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9948" yWindow="1464" windowWidth="11280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>[tblEmployee]</t>
   </si>
@@ -214,6 +214,63 @@
   </si>
   <si>
     <t>no action</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>dbo.View</t>
+  </si>
+  <si>
+    <t>dbo</t>
+  </si>
+  <si>
+    <t>database owner</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>dbo.Table1</t>
+  </si>
+  <si>
+    <t>dbo.Table2</t>
+  </si>
+  <si>
+    <t>dbo.view</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>select * from dbo.View</t>
+  </si>
+  <si>
+    <t>denied select</t>
+  </si>
+  <si>
+    <t>Have I got dbo.View?</t>
+  </si>
+  <si>
+    <t>Within dbo.View, I can access to ALL dbo objects</t>
+  </si>
+  <si>
+    <t>select * from dbo.Table1</t>
+  </si>
+  <si>
+    <t>Account.Table3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if denied select</t>
+  </si>
+  <si>
+    <t>no access with view</t>
+  </si>
+  <si>
+    <t>if ok by Account</t>
+  </si>
+  <si>
+    <t>access ok</t>
   </si>
 </sst>
 </file>
@@ -352,6 +409,318 @@
         <a:xfrm>
           <a:off x="7452360" y="624840"/>
           <a:ext cx="228600" cy="434340"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8507F2A6-8F12-44B0-8FC3-EBA6A8411FC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1394460" y="6652260"/>
+          <a:ext cx="1303020" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6CC175E-3D5D-439F-A862-BC3E47714FD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="7307580"/>
+          <a:ext cx="1181100" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C59E0D1D-62B9-4E10-8EE3-99B89B18FC7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2499360" y="7315200"/>
+          <a:ext cx="1158240" cy="350520"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>746760</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101566D0-91EC-4E82-9554-89EDB9CA19B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4655820" y="7391400"/>
+          <a:ext cx="716280" cy="15240"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>754380</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733CAE90-E37F-4E4D-8BF9-C6422858EA59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4762500" y="7597140"/>
+          <a:ext cx="617220" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9CFED6-B99B-45EA-80E5-0A8445613E84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4686300" y="7795260"/>
+          <a:ext cx="655320" cy="15240"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -701,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:P34"/>
+  <dimension ref="A3:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,7 +1424,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>60</v>
       </c>
@@ -1063,12 +1432,96 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>61</v>
       </c>
       <c r="C34" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>